<commit_message>
Added summary of results.
</commit_message>
<xml_diff>
--- a/WP_2_1/Results/CVD Mortality Rate 2017_allExposures_XY/PredictionTask_results_summary.xlsx
+++ b/WP_2_1/Results/CVD Mortality Rate 2017_allExposures_XY/PredictionTask_results_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="25">
   <si>
     <t>Method</t>
   </si>
@@ -151,6 +151,29 @@
       </rPr>
       <t xml:space="preserve"> x_mp, y_mp, foreign_17, inc_hh_17, inc_17, nondipl_17, abi_17, arbl_17, GISD_14, geb_abs, hh_abs, pers_abs, imp_pct25_18, imp_pct50_18, imp_mean_18, imp_pct75_18, imp_pct95_18, grn_pct05, grn_pct25, grn_pct50, grn_mean, grn_pct75, grn_pct95, cvd_mortality_17, noise_mean_17, NO2_pct05_17, NO2_pct25_17, NO2_pct50_17, NO2_mean_17, NO2_pct75_17, NO2_pct95_17, O3_pct05_17, O3_pct25_17, O3_pct50_17, O3_mean_17, O3_pct75_17, O3_pct95_17, PM10_pct05_17, PM10_pct25_17, PM10_pct50_17, PM10_mean_17, PM10_pct75_17, PM10_pct95_17, PM25_pct05_17, PM25_pct25_17, PM25_pct50_17, PM25_mean_17, PM25_pct75_17, PM25_pct95_17
  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Model with stability selection selected features</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: x_mp, y_mp, foreign_17, inc_hh_17, inc_17, nondipl_17, abi_17, arbl_17, GISD_14, geb_abs, hh_abs, imp_pct25_18, imp_pct50_18, imp_pct75_18, imp_pct95_18, grn_pct05, grn_pct25, grn_pct75, grn_pct95, noise_mean_17, NO2_pct05_17, O3_pct05_17, PM10_pct05_17, PM25_pct05_17</t>
     </r>
   </si>
 </sst>
@@ -294,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +497,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -650,7 +679,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,30 +687,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -704,6 +715,30 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1026,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:AF40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1064,177 +1099,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="71" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="6" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
     </row>
-    <row r="3" spans="1:32" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="14" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="14" t="s">
+      <c r="U3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="18"/>
-      <c r="W3" s="14" t="s">
+      <c r="V3" s="12"/>
+      <c r="W3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="X3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Y3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AA3" s="14" t="s">
+      <c r="AA3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="14" t="s">
+      <c r="AB3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AC3" s="14" t="s">
+      <c r="AC3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AD3" s="14" t="s">
+      <c r="AD3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AE3" s="14" t="s">
+      <c r="AE3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AF3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2">
@@ -1264,8 +1299,8 @@
       <c r="J4" s="2">
         <v>0.46200000000000002</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="14" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="2">
@@ -1295,8 +1330,8 @@
       <c r="U4" s="2">
         <v>0.46200000000000002</v>
       </c>
-      <c r="V4" s="7"/>
-      <c r="W4" s="14" t="s">
+      <c r="V4" s="4"/>
+      <c r="W4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="X4" s="2">
@@ -1328,7 +1363,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2">
@@ -1358,8 +1393,8 @@
       <c r="J5" s="2">
         <v>0.441</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="14" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="2">
@@ -1389,8 +1424,8 @@
       <c r="U5" s="2">
         <v>0.46200000000000002</v>
       </c>
-      <c r="V5" s="7"/>
-      <c r="W5" s="14" t="s">
+      <c r="V5" s="4"/>
+      <c r="W5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="X5" s="2">
@@ -1422,7 +1457,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2">
@@ -1452,8 +1487,8 @@
       <c r="J6" s="2">
         <v>0.13700000000000001</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="14" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="M6" s="2">
@@ -1483,8 +1518,8 @@
       <c r="U6" s="2">
         <v>0.45600000000000002</v>
       </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="14" t="s">
+      <c r="V6" s="4"/>
+      <c r="W6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="X6" s="2">
@@ -1516,7 +1551,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2">
@@ -1546,8 +1581,8 @@
       <c r="J7" s="2">
         <v>0.13700000000000001</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="14" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M7" s="2">
@@ -1577,8 +1612,8 @@
       <c r="U7" s="2">
         <v>0.45400000000000001</v>
       </c>
-      <c r="V7" s="7"/>
-      <c r="W7" s="14" t="s">
+      <c r="V7" s="4"/>
+      <c r="W7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="X7" s="2">
@@ -1610,7 +1645,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
@@ -1640,8 +1675,8 @@
       <c r="J8" s="2">
         <v>0.48099999999999998</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="14" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="2">
@@ -1671,8 +1706,8 @@
       <c r="U8" s="2">
         <v>0.502</v>
       </c>
-      <c r="V8" s="7"/>
-      <c r="W8" s="14" t="s">
+      <c r="V8" s="4"/>
+      <c r="W8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="X8" s="2">
@@ -1704,7 +1739,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2">
@@ -1734,8 +1769,8 @@
       <c r="J9" s="2">
         <v>0.38300000000000001</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="14" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="M9" s="2">
@@ -1765,8 +1800,8 @@
       <c r="U9" s="2">
         <v>0.41299999999999998</v>
       </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="14" t="s">
+      <c r="V9" s="4"/>
+      <c r="W9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="X9" s="2">
@@ -1798,7 +1833,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2">
@@ -1828,8 +1863,8 @@
       <c r="J10" s="2">
         <v>0.49</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="M10" s="2">
@@ -1859,8 +1894,8 @@
       <c r="U10" s="2">
         <v>0.53500000000000003</v>
       </c>
-      <c r="V10" s="7"/>
-      <c r="W10" s="14" t="s">
+      <c r="V10" s="4"/>
+      <c r="W10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="X10" s="2">
@@ -1892,7 +1927,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2">
@@ -1922,8 +1957,8 @@
       <c r="J11" s="2">
         <v>0.65900000000000003</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="14" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="M11" s="2">
@@ -1953,8 +1988,8 @@
       <c r="U11" s="2">
         <v>0.65500000000000003</v>
       </c>
-      <c r="V11" s="7"/>
-      <c r="W11" s="14" t="s">
+      <c r="V11" s="4"/>
+      <c r="W11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X11" s="2">
@@ -1986,1845 +2021,2751 @@
       </c>
     </row>
     <row r="14" spans="1:32" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="21"/>
+      <c r="AC14" s="21"/>
+      <c r="AD14" s="21"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="21"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="11" t="s">
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
     </row>
-    <row r="16" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="15" t="s">
+      <c r="K16" s="11"/>
+      <c r="L16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="15" t="s">
+      <c r="N16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="P16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Q16" s="15" t="s">
+      <c r="Q16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R16" s="15" t="s">
+      <c r="R16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S16" s="15" t="s">
+      <c r="S16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="T16" s="15" t="s">
+      <c r="T16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="U16" s="15" t="s">
+      <c r="U16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V16" s="17"/>
-      <c r="W16" s="15" t="s">
+      <c r="V16" s="11"/>
+      <c r="W16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="X16" s="15" t="s">
+      <c r="X16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Y16" s="15" t="s">
+      <c r="Y16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Z16" s="15" t="s">
+      <c r="Z16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AA16" s="15" t="s">
+      <c r="AA16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AB16" s="15" t="s">
+      <c r="AB16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AC16" s="15" t="s">
+      <c r="AC16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AD16" s="15" t="s">
+      <c r="AD16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AE16" s="15" t="s">
+      <c r="AE16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AF16" s="15" t="s">
+      <c r="AF16" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="6">
         <v>9.4E-2</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="6">
         <v>0.22</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="6">
         <v>0.91</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="6">
         <v>0.19900000000000001</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="6">
         <v>0.93</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="6">
         <v>0.52600000000000002</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="6">
         <v>0.53600000000000003</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="6">
         <v>0.48</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="15" t="s">
+      <c r="K17" s="7"/>
+      <c r="L17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="6">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="6">
         <v>0.218</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="6">
         <v>0.91</v>
       </c>
-      <c r="P17" s="12">
+      <c r="P17" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="Q17" s="6">
         <v>0.19800000000000001</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="6">
         <v>0.93</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17" s="6">
         <v>0.51700000000000002</v>
       </c>
-      <c r="T17" s="12">
+      <c r="T17" s="6">
         <v>0.53200000000000003</v>
       </c>
-      <c r="U17" s="12">
+      <c r="U17" s="6">
         <v>0.48</v>
       </c>
-      <c r="V17" s="13"/>
-      <c r="W17" s="15" t="s">
+      <c r="V17" s="7"/>
+      <c r="W17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="X17" s="12">
+      <c r="X17" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Y17" s="12">
+      <c r="Y17" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="Z17" s="12">
+      <c r="Z17" s="6">
         <v>0.91</v>
       </c>
-      <c r="AA17" s="12">
+      <c r="AA17" s="6">
         <v>2E-3</v>
       </c>
-      <c r="AB17" s="12">
+      <c r="AB17" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AC17" s="12">
+      <c r="AC17" s="6">
         <v>0.93</v>
       </c>
-      <c r="AD17" s="12">
+      <c r="AD17" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AE17" s="12">
+      <c r="AE17" s="6">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="AF17" s="12">
+      <c r="AF17" s="6">
         <v>0.48</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="6">
         <v>0.219</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="6">
         <v>0.90900000000000003</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="6">
         <v>0.19800000000000001</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="6">
         <v>0.92900000000000005</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="6">
         <v>0.54800000000000004</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="6">
         <v>0.45800000000000002</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="15" t="s">
+      <c r="K18" s="7"/>
+      <c r="L18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="12">
+      <c r="M18" s="6">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="6">
         <v>0.218</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="6">
         <v>0.91</v>
       </c>
-      <c r="P18" s="12">
+      <c r="P18" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="Q18" s="12">
+      <c r="Q18" s="6">
         <v>0.19800000000000001</v>
       </c>
-      <c r="R18" s="12">
+      <c r="R18" s="6">
         <v>0.92900000000000005</v>
       </c>
-      <c r="S18" s="12">
+      <c r="S18" s="6">
         <v>0.52200000000000002</v>
       </c>
-      <c r="T18" s="12">
+      <c r="T18" s="6">
         <v>0.53500000000000003</v>
       </c>
-      <c r="U18" s="12">
+      <c r="U18" s="6">
         <v>0.47499999999999998</v>
       </c>
-      <c r="V18" s="13"/>
-      <c r="W18" s="15" t="s">
+      <c r="V18" s="7"/>
+      <c r="W18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="X18" s="12">
+      <c r="X18" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Y18" s="12">
+      <c r="Y18" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="Z18" s="12">
+      <c r="Z18" s="6">
         <v>0.90900000000000003</v>
       </c>
-      <c r="AA18" s="12">
+      <c r="AA18" s="6">
         <v>2E-3</v>
       </c>
-      <c r="AB18" s="12">
+      <c r="AB18" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AC18" s="12">
+      <c r="AC18" s="6">
         <v>0.92800000000000005</v>
       </c>
-      <c r="AD18" s="12">
+      <c r="AD18" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AE18" s="12">
+      <c r="AE18" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="AF18" s="12">
+      <c r="AF18" s="6">
         <v>0.46600000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="6">
         <v>0.53900000000000003</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="6">
         <v>0.48499999999999999</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="6">
         <v>0.47699999999999998</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="6">
         <v>0.58199999999999996</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="6">
         <v>0.53200000000000003</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="6">
         <v>0.873</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="6">
         <v>0.13700000000000001</v>
       </c>
-      <c r="K19" s="13"/>
-      <c r="L19" s="15" t="s">
+      <c r="K19" s="7"/>
+      <c r="L19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="6">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="6">
         <v>0.218</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="6">
         <v>0.91</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P19" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q19" s="12">
+      <c r="Q19" s="6">
         <v>0.19700000000000001</v>
       </c>
-      <c r="R19" s="12">
+      <c r="R19" s="6">
         <v>0.93</v>
       </c>
-      <c r="S19" s="12">
+      <c r="S19" s="6">
         <v>0.52500000000000002</v>
       </c>
-      <c r="T19" s="12">
+      <c r="T19" s="6">
         <v>0.53700000000000003</v>
       </c>
-      <c r="U19" s="12">
+      <c r="U19" s="6">
         <v>0.47299999999999998</v>
       </c>
-      <c r="V19" s="13"/>
-      <c r="W19" s="15" t="s">
+      <c r="V19" s="7"/>
+      <c r="W19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X19" s="12">
+      <c r="X19" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Y19" s="12">
+      <c r="Y19" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="Z19" s="12">
+      <c r="Z19" s="6">
         <v>0.91</v>
       </c>
-      <c r="AA19" s="12">
+      <c r="AA19" s="6">
         <v>2E-3</v>
       </c>
-      <c r="AB19" s="12">
+      <c r="AB19" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AC19" s="12">
+      <c r="AC19" s="6">
         <v>0.93</v>
       </c>
-      <c r="AD19" s="12">
+      <c r="AD19" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AE19" s="12">
+      <c r="AE19" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="AF19" s="12">
+      <c r="AF19" s="6">
         <v>0.47199999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="6">
         <v>0.53900000000000003</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="6">
         <v>0.60299999999999998</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="6">
         <v>0.48499999999999999</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="6">
         <v>0.47699999999999998</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="6">
         <v>0.58199999999999996</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="6">
         <v>0.53200000000000003</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="6">
         <v>0.873</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="6">
         <v>0.13700000000000001</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="15" t="s">
+      <c r="K20" s="7"/>
+      <c r="L20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="12">
+      <c r="M20" s="6">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="6">
         <v>0.218</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="6">
         <v>0.91</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="Q20" s="12">
+      <c r="Q20" s="6">
         <v>0.19800000000000001</v>
       </c>
-      <c r="R20" s="12">
+      <c r="R20" s="6">
         <v>0.93</v>
       </c>
-      <c r="S20" s="12">
+      <c r="S20" s="6">
         <v>0.52700000000000002</v>
       </c>
-      <c r="T20" s="12">
+      <c r="T20" s="6">
         <v>0.53900000000000003</v>
       </c>
-      <c r="U20" s="12">
+      <c r="U20" s="6">
         <v>0.47</v>
       </c>
-      <c r="V20" s="13"/>
-      <c r="W20" s="15" t="s">
+      <c r="V20" s="7"/>
+      <c r="W20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X20" s="12">
+      <c r="X20" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Y20" s="12">
+      <c r="Y20" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="Z20" s="12">
+      <c r="Z20" s="6">
         <v>0.90900000000000003</v>
       </c>
-      <c r="AA20" s="12">
+      <c r="AA20" s="6">
         <v>2E-3</v>
       </c>
-      <c r="AB20" s="12">
+      <c r="AB20" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AC20" s="12">
+      <c r="AC20" s="6">
         <v>0.93</v>
       </c>
-      <c r="AD20" s="12">
+      <c r="AD20" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AE20" s="12">
+      <c r="AE20" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="AF20" s="12">
+      <c r="AF20" s="6">
         <v>0.46800000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="6">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="6">
         <v>0.99399999999999999</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="6">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="6">
         <v>0.98099999999999998</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="6">
         <v>0.41</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="6">
         <v>0.5</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="6">
         <v>0.59499999999999997</v>
       </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="15" t="s">
+      <c r="K21" s="7"/>
+      <c r="L21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M21" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="6">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="6">
         <v>0.99399999999999999</v>
       </c>
-      <c r="P21" s="12">
+      <c r="P21" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="Q21" s="12">
+      <c r="Q21" s="6">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="6">
         <v>0.98099999999999998</v>
       </c>
-      <c r="S21" s="12">
+      <c r="S21" s="6">
         <v>0.40300000000000002</v>
       </c>
-      <c r="T21" s="12">
+      <c r="T21" s="6">
         <v>0.496</v>
       </c>
-      <c r="U21" s="12">
+      <c r="U21" s="6">
         <v>0.59499999999999997</v>
       </c>
-      <c r="V21" s="13"/>
-      <c r="W21" s="15" t="s">
+      <c r="V21" s="7"/>
+      <c r="W21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X21" s="12">
+      <c r="X21" s="6">
         <v>0</v>
       </c>
-      <c r="Y21" s="12">
+      <c r="Y21" s="6">
         <v>0.01</v>
       </c>
-      <c r="Z21" s="12">
+      <c r="Z21" s="6">
         <v>0.99399999999999999</v>
       </c>
-      <c r="AA21" s="12">
+      <c r="AA21" s="6">
         <v>1E-3</v>
       </c>
-      <c r="AB21" s="12">
+      <c r="AB21" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="AC21" s="12">
+      <c r="AC21" s="6">
         <v>0.98099999999999998</v>
       </c>
-      <c r="AD21" s="12">
+      <c r="AD21" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AE21" s="12">
+      <c r="AE21" s="6">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="AF21" s="12">
+      <c r="AF21" s="6">
         <v>0.59499999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="6">
         <v>0.99299999999999999</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="6">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="6">
         <v>0.98499999999999999</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="6">
         <v>0.42499999999999999</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="6">
         <v>0.48099999999999998</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="15" t="s">
+      <c r="K22" s="7"/>
+      <c r="L22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="6">
         <v>0.99099999999999999</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="6">
         <v>0.02</v>
       </c>
-      <c r="Q22" s="12">
+      <c r="Q22" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="6">
         <v>0.98</v>
       </c>
-      <c r="S22" s="12">
+      <c r="S22" s="6">
         <v>0.41599999999999998</v>
       </c>
-      <c r="T22" s="12">
+      <c r="T22" s="6">
         <v>0.47799999999999998</v>
       </c>
-      <c r="U22" s="12">
+      <c r="U22" s="6">
         <v>0.58099999999999996</v>
       </c>
-      <c r="V22" s="13"/>
-      <c r="W22" s="15" t="s">
+      <c r="V22" s="7"/>
+      <c r="W22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="X22" s="12">
+      <c r="X22" s="6">
         <v>0</v>
       </c>
-      <c r="Y22" s="12">
+      <c r="Y22" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="Z22" s="12">
+      <c r="Z22" s="6">
         <v>0.99199999999999999</v>
       </c>
-      <c r="AA22" s="12">
+      <c r="AA22" s="6">
         <v>1E-3</v>
       </c>
-      <c r="AB22" s="12">
+      <c r="AB22" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AC22" s="12">
+      <c r="AC22" s="6">
         <v>0.98</v>
       </c>
-      <c r="AD22" s="12">
+      <c r="AD22" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="AE22" s="12">
+      <c r="AE22" s="6">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="AF22" s="12">
+      <c r="AF22" s="6">
         <v>0.56499999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="6">
         <v>0.159</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="6">
         <v>0.95899999999999996</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="6">
         <v>4.7E-2</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="6">
         <v>0.16200000000000001</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="6">
         <v>0.95399999999999996</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="6">
         <v>0.47699999999999998</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="6">
         <v>0.53600000000000003</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="6">
         <v>0.52800000000000002</v>
       </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="15" t="s">
+      <c r="K23" s="7"/>
+      <c r="L23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="6">
         <v>0.158</v>
       </c>
-      <c r="O23" s="12">
+      <c r="O23" s="6">
         <v>0.95899999999999996</v>
       </c>
-      <c r="P23" s="12">
+      <c r="P23" s="6">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="Q23" s="12">
+      <c r="Q23" s="6">
         <v>0.16</v>
       </c>
-      <c r="R23" s="12">
+      <c r="R23" s="6">
         <v>0.95399999999999996</v>
       </c>
-      <c r="S23" s="12">
+      <c r="S23" s="6">
         <v>0.46300000000000002</v>
       </c>
-      <c r="T23" s="12">
+      <c r="T23" s="6">
         <v>0.52900000000000003</v>
       </c>
-      <c r="U23" s="12">
+      <c r="U23" s="6">
         <v>0.53400000000000003</v>
       </c>
-      <c r="V23" s="13"/>
-      <c r="W23" s="15" t="s">
+      <c r="V23" s="7"/>
+      <c r="W23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="X23" s="12">
+      <c r="X23" s="6">
         <v>2E-3</v>
       </c>
-      <c r="Y23" s="12">
+      <c r="Y23" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="Z23" s="12">
+      <c r="Z23" s="6">
         <v>0.95399999999999996</v>
       </c>
-      <c r="AA23" s="12">
+      <c r="AA23" s="6">
         <v>2E-3</v>
       </c>
-      <c r="AB23" s="12">
+      <c r="AB23" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="AC23" s="12">
+      <c r="AC23" s="6">
         <v>0.93600000000000005</v>
       </c>
-      <c r="AD23" s="12">
+      <c r="AD23" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AE23" s="12">
+      <c r="AE23" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AF23" s="12">
+      <c r="AF23" s="6">
         <v>0.53200000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="6">
         <v>0</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="6">
         <v>1</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="6">
         <v>0.06</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="6">
         <v>0.98399999999999999</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="6">
         <v>0.41699999999999998</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="6">
         <v>0.47699999999999998</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="6">
         <v>0.58799999999999997</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="15" t="s">
+      <c r="K24" s="7"/>
+      <c r="L24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="12">
+      <c r="M24" s="6">
         <v>0</v>
       </c>
-      <c r="N24" s="12">
+      <c r="N24" s="6">
         <v>1E-3</v>
       </c>
-      <c r="O24" s="12">
+      <c r="O24" s="6">
         <v>1</v>
       </c>
-      <c r="P24" s="12">
+      <c r="P24" s="6">
         <v>0.02</v>
       </c>
-      <c r="Q24" s="12">
+      <c r="Q24" s="6">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="R24" s="12">
+      <c r="R24" s="6">
         <v>0.98</v>
       </c>
-      <c r="S24" s="12">
+      <c r="S24" s="6">
         <v>0.34899999999999998</v>
       </c>
-      <c r="T24" s="12">
+      <c r="T24" s="6">
         <v>0.436</v>
       </c>
-      <c r="U24" s="12">
+      <c r="U24" s="6">
         <v>0.64900000000000002</v>
       </c>
-      <c r="V24" s="13"/>
-      <c r="W24" s="15" t="s">
+      <c r="V24" s="7"/>
+      <c r="W24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="X24" s="12">
+      <c r="X24" s="6">
         <v>0</v>
       </c>
-      <c r="Y24" s="12">
+      <c r="Y24" s="6">
         <v>1E-3</v>
       </c>
-      <c r="Z24" s="12">
+      <c r="Z24" s="6">
         <v>1</v>
       </c>
-      <c r="AA24" s="12">
+      <c r="AA24" s="6">
         <v>1E-3</v>
       </c>
-      <c r="AB24" s="12">
+      <c r="AB24" s="6">
         <v>0.01</v>
       </c>
-      <c r="AC24" s="12">
+      <c r="AC24" s="6">
         <v>0.98199999999999998</v>
       </c>
-      <c r="AD24" s="12">
+      <c r="AD24" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="AE24" s="12">
+      <c r="AE24" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="AF24" s="12">
+      <c r="AF24" s="6">
         <v>0.66300000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="8"/>
-      <c r="AB27" s="8"/>
-      <c r="AC27" s="8"/>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="21"/>
+      <c r="AC27" s="21"/>
+      <c r="AD27" s="21"/>
+      <c r="AE27" s="21"/>
+      <c r="AF27" s="21"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="11" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="10"/>
-      <c r="W28" s="11" t="s">
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
-      <c r="AD28" s="11"/>
-      <c r="AE28" s="11"/>
-      <c r="AF28" s="11"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="16"/>
+      <c r="AB28" s="16"/>
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="16"/>
     </row>
-    <row r="29" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="M29" s="15" t="s">
+      <c r="M29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N29" s="15" t="s">
+      <c r="N29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O29" s="15" t="s">
+      <c r="O29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P29" s="15" t="s">
+      <c r="P29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Q29" s="15" t="s">
+      <c r="Q29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R29" s="15" t="s">
+      <c r="R29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S29" s="15" t="s">
+      <c r="S29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="T29" s="15" t="s">
+      <c r="T29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="U29" s="15" t="s">
+      <c r="U29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="W29" s="15" t="s">
+      <c r="W29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="X29" s="15" t="s">
+      <c r="X29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Y29" s="15" t="s">
+      <c r="Y29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Z29" s="15" t="s">
+      <c r="Z29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AA29" s="15" t="s">
+      <c r="AA29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AB29" s="15" t="s">
+      <c r="AB29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AC29" s="15" t="s">
+      <c r="AC29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AD29" s="15" t="s">
+      <c r="AD29" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AE29" s="15" t="s">
+      <c r="AE29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AF29" s="15" t="s">
+      <c r="AF29" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="6">
         <v>0.13500000000000001</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="6">
         <v>0.26800000000000002</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="6">
         <v>0.871</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="6">
         <v>0.23300000000000001</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="6">
         <v>0.90300000000000002</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="6">
         <v>0.80200000000000005</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="6">
         <v>0.67200000000000004</v>
       </c>
-      <c r="J30" s="12">
+      <c r="J30" s="6">
         <v>0.20699999999999999</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M30" s="12">
+      <c r="M30" s="6">
         <v>0.13200000000000001</v>
       </c>
-      <c r="N30" s="12">
+      <c r="N30" s="6">
         <v>0.26600000000000001</v>
       </c>
-      <c r="O30" s="12">
+      <c r="O30" s="6">
         <v>0.871</v>
       </c>
-      <c r="P30" s="12">
+      <c r="P30" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="Q30" s="12">
+      <c r="Q30" s="6">
         <v>0.23100000000000001</v>
       </c>
-      <c r="R30" s="12">
+      <c r="R30" s="6">
         <v>0.90300000000000002</v>
       </c>
-      <c r="S30" s="12">
+      <c r="S30" s="6">
         <v>0.78900000000000003</v>
       </c>
-      <c r="T30" s="12">
+      <c r="T30" s="6">
         <v>0.66600000000000004</v>
       </c>
-      <c r="U30" s="12">
+      <c r="U30" s="6">
         <v>0.20699999999999999</v>
       </c>
-      <c r="W30" s="15" t="s">
+      <c r="W30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="X30" s="12">
+      <c r="X30" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Y30" s="12">
+      <c r="Y30" s="6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="Z30" s="12">
+      <c r="Z30" s="6">
         <v>0.871</v>
       </c>
-      <c r="AA30" s="12">
+      <c r="AA30" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AB30" s="12">
+      <c r="AB30" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="AC30" s="12">
+      <c r="AC30" s="6">
         <v>0.90300000000000002</v>
       </c>
-      <c r="AD30" s="12">
+      <c r="AD30" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AE30" s="12">
+      <c r="AE30" s="6">
         <v>0.12</v>
       </c>
-      <c r="AF30" s="12">
+      <c r="AF30" s="6">
         <v>0.20699999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="6">
         <v>0.13500000000000001</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="6">
         <v>0.26800000000000002</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="6">
         <v>0.871</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="6">
         <v>0.23300000000000001</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="6">
         <v>0.90400000000000003</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="6">
         <v>0.8</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="6">
         <v>0.67100000000000004</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="6">
         <v>0.20899999999999999</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="12">
+      <c r="M31" s="6">
         <v>0.13200000000000001</v>
       </c>
-      <c r="N31" s="12">
+      <c r="N31" s="6">
         <v>0.26600000000000001</v>
       </c>
-      <c r="O31" s="12">
+      <c r="O31" s="6">
         <v>0.871</v>
       </c>
-      <c r="P31" s="12">
+      <c r="P31" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="Q31" s="12">
+      <c r="Q31" s="6">
         <v>0.23100000000000001</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R31" s="6">
         <v>0.90300000000000002</v>
       </c>
-      <c r="S31" s="12">
+      <c r="S31" s="6">
         <v>0.78900000000000003</v>
       </c>
-      <c r="T31" s="12">
+      <c r="T31" s="6">
         <v>0.66600000000000004</v>
       </c>
-      <c r="U31" s="12">
+      <c r="U31" s="6">
         <v>0.20699999999999999</v>
       </c>
-      <c r="W31" s="15" t="s">
+      <c r="W31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="X31" s="12">
+      <c r="X31" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Y31" s="12">
+      <c r="Y31" s="6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="Z31" s="12">
+      <c r="Z31" s="6">
         <v>0.871</v>
       </c>
-      <c r="AA31" s="12">
+      <c r="AA31" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AB31" s="12">
+      <c r="AB31" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="AC31" s="12">
+      <c r="AC31" s="6">
         <v>0.9</v>
       </c>
-      <c r="AD31" s="12">
+      <c r="AD31" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE31" s="12">
+      <c r="AE31" s="6">
         <v>0.11799999999999999</v>
       </c>
-      <c r="AF31" s="12">
+      <c r="AF31" s="6">
         <v>0.23100000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="6">
         <v>0.54400000000000004</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="6">
         <v>0.60899999999999999</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="6">
         <v>0.48099999999999998</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="6">
         <v>0.47899999999999998</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="6">
         <v>0.58399999999999996</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="6">
         <v>0.53</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="6">
         <v>0.874</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="6">
         <v>0.13600000000000001</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="6">
         <v>0.13300000000000001</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="6">
         <v>0.26700000000000002</v>
       </c>
-      <c r="O32" s="12">
+      <c r="O32" s="6">
         <v>0.871</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="Q32" s="12">
+      <c r="Q32" s="6">
         <v>0.23300000000000001</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="6">
         <v>0.90300000000000002</v>
       </c>
-      <c r="S32" s="12">
+      <c r="S32" s="6">
         <v>0.77900000000000003</v>
       </c>
-      <c r="T32" s="12">
+      <c r="T32" s="6">
         <v>0.66200000000000003</v>
       </c>
-      <c r="U32" s="12">
+      <c r="U32" s="6">
         <v>0.217</v>
       </c>
-      <c r="W32" s="15" t="s">
+      <c r="W32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X32" s="12">
+      <c r="X32" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Y32" s="12">
+      <c r="Y32" s="6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="Z32" s="12">
+      <c r="Z32" s="6">
         <v>0.871</v>
       </c>
-      <c r="AA32" s="12">
+      <c r="AA32" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AB32" s="12">
+      <c r="AB32" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="AC32" s="12">
+      <c r="AC32" s="6">
         <v>0.90300000000000002</v>
       </c>
-      <c r="AD32" s="12">
+      <c r="AD32" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE32" s="12">
+      <c r="AE32" s="6">
         <v>0.11899999999999999</v>
       </c>
-      <c r="AF32" s="12">
+      <c r="AF32" s="6">
         <v>0.219</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="6">
         <v>0.54400000000000004</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="6">
         <v>0.60899999999999999</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="6">
         <v>0.48099999999999998</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="6">
         <v>0.47899999999999998</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="6">
         <v>0.58399999999999996</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="6">
         <v>0.53</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="6">
         <v>0.874</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="J33" s="12">
+      <c r="J33" s="6">
         <v>0.13600000000000001</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="L33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M33" s="12">
+      <c r="M33" s="6">
         <v>0.13300000000000001</v>
       </c>
-      <c r="N33" s="12">
+      <c r="N33" s="6">
         <v>0.26700000000000002</v>
       </c>
-      <c r="O33" s="12">
+      <c r="O33" s="6">
         <v>0.871</v>
       </c>
-      <c r="P33" s="12">
+      <c r="P33" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="Q33" s="12">
+      <c r="Q33" s="6">
         <v>0.23400000000000001</v>
       </c>
-      <c r="R33" s="12">
+      <c r="R33" s="6">
         <v>0.90200000000000002</v>
       </c>
-      <c r="S33" s="12">
+      <c r="S33" s="6">
         <v>0.77600000000000002</v>
       </c>
-      <c r="T33" s="12">
+      <c r="T33" s="6">
         <v>0.66100000000000003</v>
       </c>
-      <c r="U33" s="12">
+      <c r="U33" s="6">
         <v>0.22</v>
       </c>
-      <c r="W33" s="15" t="s">
+      <c r="W33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X33" s="12">
+      <c r="X33" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Y33" s="12">
+      <c r="Y33" s="6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="Z33" s="12">
+      <c r="Z33" s="6">
         <v>0.871</v>
       </c>
-      <c r="AA33" s="12">
+      <c r="AA33" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AB33" s="12">
+      <c r="AB33" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="AC33" s="12">
+      <c r="AC33" s="6">
         <v>0.90200000000000002</v>
       </c>
-      <c r="AD33" s="12">
+      <c r="AD33" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE33" s="12">
+      <c r="AE33" s="6">
         <v>0.11899999999999999</v>
       </c>
-      <c r="AF33" s="12">
+      <c r="AF33" s="6">
         <v>0.224</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="6">
         <v>0.02</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="6">
         <v>0.98099999999999998</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="6">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="6">
         <v>0.108</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="6">
         <v>0.98</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="6">
         <v>0.70099999999999996</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="6">
         <v>0.59</v>
       </c>
-      <c r="J34" s="12">
+      <c r="J34" s="6">
         <v>0.307</v>
       </c>
-      <c r="L34" s="15" t="s">
+      <c r="L34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M34" s="12">
+      <c r="M34" s="6">
         <v>0.02</v>
       </c>
-      <c r="N34" s="12">
+      <c r="N34" s="6">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="O34" s="12">
+      <c r="O34" s="6">
         <v>0.98099999999999998</v>
       </c>
-      <c r="P34" s="12">
+      <c r="P34" s="6">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="Q34" s="12">
+      <c r="Q34" s="6">
         <v>0.107</v>
       </c>
-      <c r="R34" s="12">
+      <c r="R34" s="6">
         <v>0.98</v>
       </c>
-      <c r="S34" s="12">
+      <c r="S34" s="6">
         <v>0.68899999999999995</v>
       </c>
-      <c r="T34" s="12">
+      <c r="T34" s="6">
         <v>0.58499999999999996</v>
       </c>
-      <c r="U34" s="12">
+      <c r="U34" s="6">
         <v>0.307</v>
       </c>
-      <c r="W34" s="15" t="s">
+      <c r="W34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="X34" s="12">
+      <c r="X34" s="6">
         <v>1E-3</v>
       </c>
-      <c r="Y34" s="12">
+      <c r="Y34" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="Z34" s="12">
+      <c r="Z34" s="6">
         <v>0.98099999999999998</v>
       </c>
-      <c r="AA34" s="12">
+      <c r="AA34" s="6">
         <v>1E-3</v>
       </c>
-      <c r="AB34" s="12">
+      <c r="AB34" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="AC34" s="12">
+      <c r="AC34" s="6">
         <v>0.98</v>
       </c>
-      <c r="AD34" s="12">
+      <c r="AD34" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="AE34" s="12">
+      <c r="AE34" s="6">
         <v>0.105</v>
       </c>
-      <c r="AF34" s="12">
+      <c r="AF34" s="6">
         <v>0.307</v>
       </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="6">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="6">
         <v>0.99</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="6">
         <v>0.1</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="6">
         <v>0.97299999999999998</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="6">
         <v>0.53500000000000003</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="6">
         <v>0.53400000000000003</v>
       </c>
-      <c r="J35" s="12">
+      <c r="J35" s="6">
         <v>0.47099999999999997</v>
       </c>
-      <c r="L35" s="15" t="s">
+      <c r="L35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M35" s="12">
+      <c r="M35" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N35" s="12">
+      <c r="N35" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="O35" s="12">
+      <c r="O35" s="6">
         <v>0.99199999999999999</v>
       </c>
-      <c r="P35" s="12">
+      <c r="P35" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="Q35" s="12">
+      <c r="Q35" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="R35" s="12">
+      <c r="R35" s="6">
         <v>0.97</v>
       </c>
-      <c r="S35" s="12">
+      <c r="S35" s="6">
         <v>0.47699999999999998</v>
       </c>
-      <c r="T35" s="12">
+      <c r="T35" s="6">
         <v>0.51</v>
       </c>
-      <c r="U35" s="12">
+      <c r="U35" s="6">
         <v>0.52100000000000002</v>
       </c>
-      <c r="W35" s="15" t="s">
+      <c r="W35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="X35" s="12">
+      <c r="X35" s="6">
         <v>0</v>
       </c>
-      <c r="Y35" s="12">
+      <c r="Y35" s="6">
         <v>0.01</v>
       </c>
-      <c r="Z35" s="12">
+      <c r="Z35" s="6">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AA35" s="12">
+      <c r="AA35" s="6">
         <v>1E-3</v>
       </c>
-      <c r="AB35" s="12">
+      <c r="AB35" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="AC35" s="12">
+      <c r="AC35" s="6">
         <v>0.96699999999999997</v>
       </c>
-      <c r="AD35" s="12">
+      <c r="AD35" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="AE35" s="12">
+      <c r="AE35" s="6">
         <v>9.4E-2</v>
       </c>
-      <c r="AF35" s="12">
+      <c r="AF35" s="6">
         <v>0.499</v>
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="6">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="6">
         <v>0.16700000000000001</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="6">
         <v>0.94799999999999995</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="6">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="6">
         <v>0.19600000000000001</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="6">
         <v>0.92700000000000005</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="6">
         <v>0.46800000000000003</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="6">
         <v>0.52900000000000003</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="6">
         <v>0.53800000000000003</v>
       </c>
-      <c r="L36" s="15" t="s">
+      <c r="L36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M36" s="12">
+      <c r="M36" s="6">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="N36" s="12">
+      <c r="N36" s="6">
         <v>0.17</v>
       </c>
-      <c r="O36" s="12">
+      <c r="O36" s="6">
         <v>0.94499999999999995</v>
       </c>
-      <c r="P36" s="12">
+      <c r="P36" s="6">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="Q36" s="12">
+      <c r="Q36" s="6">
         <v>0.19600000000000001</v>
       </c>
-      <c r="R36" s="12">
+      <c r="R36" s="6">
         <v>0.92400000000000004</v>
       </c>
-      <c r="S36" s="12">
+      <c r="S36" s="6">
         <v>0.46100000000000002</v>
       </c>
-      <c r="T36" s="12">
+      <c r="T36" s="6">
         <v>0.52100000000000002</v>
       </c>
-      <c r="U36" s="12">
+      <c r="U36" s="6">
         <v>0.53700000000000003</v>
       </c>
-      <c r="W36" s="15" t="s">
+      <c r="W36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="X36" s="12">
+      <c r="X36" s="6">
         <v>2E-3</v>
       </c>
-      <c r="Y36" s="12">
+      <c r="Y36" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="Z36" s="12">
+      <c r="Z36" s="6">
         <v>0.94399999999999995</v>
       </c>
-      <c r="AA36" s="12">
+      <c r="AA36" s="6">
         <v>2E-3</v>
       </c>
-      <c r="AB36" s="12">
+      <c r="AB36" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AC36" s="12">
+      <c r="AC36" s="6">
         <v>0.92700000000000005</v>
       </c>
-      <c r="AD36" s="12">
+      <c r="AD36" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AE36" s="12">
+      <c r="AE36" s="6">
         <v>9.4E-2</v>
       </c>
-      <c r="AF36" s="12">
+      <c r="AF36" s="6">
         <v>0.54200000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="6">
         <v>0</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="6">
         <v>1</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="6">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="6">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H37" s="6">
         <v>0.442</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="6">
         <v>0.48799999999999999</v>
       </c>
-      <c r="J37" s="12">
+      <c r="J37" s="6">
         <v>0.56299999999999994</v>
       </c>
-      <c r="L37" s="15" t="s">
+      <c r="L37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="12">
+      <c r="M37" s="6">
         <v>0</v>
       </c>
-      <c r="N37" s="12">
+      <c r="N37" s="6">
         <v>1E-3</v>
       </c>
-      <c r="O37" s="12">
+      <c r="O37" s="6">
         <v>1</v>
       </c>
-      <c r="P37" s="12">
+      <c r="P37" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="Q37" s="12">
+      <c r="Q37" s="6">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="R37" s="12">
+      <c r="R37" s="6">
         <v>0.97799999999999998</v>
       </c>
-      <c r="S37" s="12">
+      <c r="S37" s="6">
         <v>0.44900000000000001</v>
       </c>
-      <c r="T37" s="12">
+      <c r="T37" s="6">
         <v>0.505</v>
       </c>
-      <c r="U37" s="12">
+      <c r="U37" s="6">
         <v>0.54800000000000004</v>
       </c>
-      <c r="W37" s="15" t="s">
+      <c r="W37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="X37" s="12">
+      <c r="X37" s="6">
         <v>0</v>
       </c>
-      <c r="Y37" s="12">
+      <c r="Y37" s="6">
         <v>1E-3</v>
       </c>
-      <c r="Z37" s="12">
+      <c r="Z37" s="6">
         <v>1</v>
       </c>
-      <c r="AA37" s="12">
+      <c r="AA37" s="6">
         <v>1E-3</v>
       </c>
-      <c r="AB37" s="12">
+      <c r="AB37" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="AC37" s="12">
+      <c r="AC37" s="6">
         <v>0.97799999999999998</v>
       </c>
-      <c r="AD37" s="12">
+      <c r="AD37" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AE37" s="12">
+      <c r="AE37" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="AF37" s="12">
+      <c r="AF37" s="6">
         <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="21"/>
+      <c r="Z40" s="21"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="21"/>
+      <c r="AD40" s="21"/>
+      <c r="AE40" s="21"/>
+      <c r="AF40" s="21"/>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="L41" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="W41" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="16"/>
+      <c r="AC41" s="16"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N42" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O42" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="R42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="W42" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="X42" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z42" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF42" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="6">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0.216</v>
+      </c>
+      <c r="D43" s="6">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="E43" s="6">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F43" s="6">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="H43" s="6">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="I43" s="6">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="J43" s="6">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="L43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M43" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="N43" s="6">
+        <v>0.214</v>
+      </c>
+      <c r="O43" s="6">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="P43" s="6">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Q43" s="6">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="R43" s="6">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="S43" s="6">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="T43" s="6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="U43" s="6">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="W43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="X43" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Y43" s="6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Z43" s="6">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="AA43" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="AB43" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC43" s="6">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="AD43" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AE43" s="6">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="AF43" s="6">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0.215</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="E44" s="6">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F44" s="6">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="H44" s="6">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I44" s="6">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="J44" s="6">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M44" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="N44" s="6">
+        <v>0.214</v>
+      </c>
+      <c r="O44" s="6">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="P44" s="6">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="R44" s="6">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="S44" s="6">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="T44" s="6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="U44" s="6">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="W44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="X44" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Y44" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="Z44" s="6">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AA44" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="AB44" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC44" s="6">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AD44" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AE44" s="6">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AF44" s="6">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="D45" s="6">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="E45" s="6">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F45" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="H45" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="I45" s="6">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J45" s="6">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M45" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="N45" s="6">
+        <v>0.215</v>
+      </c>
+      <c r="O45" s="6">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="P45" s="6">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="R45" s="6">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="S45" s="6">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="T45" s="6">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="U45" s="6">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="W45" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="X45" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Y45" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="Z45" s="6">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AA45" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="AB45" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC45" s="6">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="AD45" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AE45" s="6">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AF45" s="6">
+        <v>0.46700000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A46" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="6">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="D46" s="6">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="E46" s="6">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F46" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="H46" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="I46" s="6">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J46" s="6">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M46" s="6">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="N46" s="6">
+        <v>0.215</v>
+      </c>
+      <c r="O46" s="6">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="P46" s="6">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="R46" s="6">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="S46" s="6">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="T46" s="6">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="U46" s="6">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="W46" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X46" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Y46" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="Z46" s="6">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AA46" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="AB46" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC46" s="6">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="AD46" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AE46" s="6">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AF46" s="6">
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A47" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C47" s="6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D47" s="6">
+        <v>0.995</v>
+      </c>
+      <c r="E47" s="6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F47" s="6">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="H47" s="6">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="I47" s="6">
+        <v>0.502</v>
+      </c>
+      <c r="J47" s="6">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M47" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="N47" s="6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="O47" s="6">
+        <v>0.995</v>
+      </c>
+      <c r="P47" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="R47" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="S47" s="6">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="T47" s="6">
+        <v>0.498</v>
+      </c>
+      <c r="U47" s="6">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="W47" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="X47" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="Z47" s="6">
+        <v>0.995</v>
+      </c>
+      <c r="AA47" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="AB47" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AC47" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="AD47" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AE47" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="AF47" s="6">
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="6">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6">
+        <v>1</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F48" s="6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="H48" s="6">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="I48" s="6">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="J48" s="6">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="L48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M48" s="6">
+        <v>0</v>
+      </c>
+      <c r="N48" s="6">
+        <v>0</v>
+      </c>
+      <c r="O48" s="6">
+        <v>1</v>
+      </c>
+      <c r="P48" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="Q48" s="6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="R48" s="6">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="S48" s="6">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="T48" s="6">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="U48" s="6">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="W48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="X48" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA48" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="AC48" s="6">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="AD48" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AE48" s="6">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AF48" s="6">
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C49" s="6">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D49" s="6">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="E49" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F49" s="6">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="H49" s="6">
+        <v>0.373</v>
+      </c>
+      <c r="I49" s="6">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="J49" s="6">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="L49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="N49" s="6">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="O49" s="6">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="P49" s="6">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="R49" s="6">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="S49" s="6">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="T49" s="6">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="U49" s="6">
+        <v>0.629</v>
+      </c>
+      <c r="W49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X49" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="Y49" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z49" s="6">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="AA49" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="AB49" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="AC49" s="6">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="AD49" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AE49" s="6">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AF49" s="6">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="6">
+        <v>0</v>
+      </c>
+      <c r="C50" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D50" s="6">
+        <v>1</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F50" s="6">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H50" s="6">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="I50" s="6">
+        <v>0.443</v>
+      </c>
+      <c r="J50" s="6">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="L50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M50" s="6">
+        <v>0</v>
+      </c>
+      <c r="N50" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="O50" s="6">
+        <v>1</v>
+      </c>
+      <c r="P50" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="R50" s="6">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="S50" s="6">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="T50" s="6">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="U50" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="W50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="X50" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA50" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AC50" s="6">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="AD50" s="6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AE50" s="6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AF50" s="6">
+        <v>0.66100000000000003</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A40:AF40"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="W41:AF41"/>
+    <mergeCell ref="L41:U41"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="A27:AF27"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="W2:AF2"/>
     <mergeCell ref="A28:J28"/>
     <mergeCell ref="L28:U28"/>
     <mergeCell ref="W28:AF28"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="L15:U15"/>
     <mergeCell ref="W15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="A27:AF27"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="L2:U2"/>
-    <mergeCell ref="W2:AF2"/>
-    <mergeCell ref="A1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>